<commit_message>
200 epoch train, and cm
</commit_message>
<xml_diff>
--- a/media/dataset_distribution.xlsx
+++ b/media/dataset_distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvin\Documents\GitHub\SoftwareDissertation\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0D3414-E241-4BC4-8F09-92FD9CEB875F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A3E5AF-2CAB-441B-9C56-4812440B213F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="2025" windowWidth="17280" windowHeight="9000" xr2:uid="{5A634DFE-2E40-48B4-941D-BCCC518AD939}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{5A634DFE-2E40-48B4-941D-BCCC518AD939}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>Train</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>1st iteration - 70/30 split</t>
+  </si>
+  <si>
+    <t>3rd iteration - 60/20/20 split</t>
   </si>
 </sst>
 </file>
@@ -420,20 +423,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A70554-815B-442B-91BE-D79E2B4633AC}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -447,7 +450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -462,7 +465,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -477,7 +480,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -492,7 +495,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -507,7 +510,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -522,7 +525,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
         <f>SUM(B3:B7)</f>
         <v>318</v>
@@ -540,12 +543,12 @@
         <v>458</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -559,7 +562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -577,7 +580,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -595,7 +598,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -613,7 +616,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -631,7 +634,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -649,7 +652,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B17">
         <f>SUM(B12:B16)</f>
         <v>739</v>
@@ -664,6 +667,140 @@
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <f>296/2</f>
+        <v>148</v>
+      </c>
+      <c r="C21">
+        <f>98/2</f>
+        <v>49</v>
+      </c>
+      <c r="D21">
+        <v>51</v>
+      </c>
+      <c r="E21">
+        <f>SUM(B21:D21)</f>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <f>308/2</f>
+        <v>154</v>
+      </c>
+      <c r="C22">
+        <f>102/2</f>
+        <v>51</v>
+      </c>
+      <c r="D22">
+        <v>52</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22:E26" si="2">SUM(B22:D22)</f>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <f>242/2</f>
+        <v>121</v>
+      </c>
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>41</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <f>244/2</f>
+        <v>122</v>
+      </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>42</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <f>272/2</f>
+        <v>136</v>
+      </c>
+      <c r="C25">
+        <v>45</v>
+      </c>
+      <c r="D25">
+        <v>47</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26">
+        <f>SUM(B21:B25)</f>
+        <v>681</v>
+      </c>
+      <c r="C26">
+        <f>SUM(C21:C25)</f>
+        <v>225</v>
+      </c>
+      <c r="D26">
+        <f>SUM(D21:D25)</f>
+        <v>233</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
         <v>1139</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final submission before adding paper
</commit_message>
<xml_diff>
--- a/media/dataset_distribution.xlsx
+++ b/media/dataset_distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvin\Documents\GitHub\SoftwareDissertation\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassa\Documents\Github\SoftwareDissertation\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2AD7A5-087D-48D3-95C2-2CC59291A5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9243D7E1-0AE0-40B0-8C84-CF232D12B3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3648" yWindow="3366" windowWidth="17280" windowHeight="8994" xr2:uid="{5A634DFE-2E40-48B4-941D-BCCC518AD939}"/>
+    <workbookView xWindow="6330" yWindow="1905" windowWidth="21600" windowHeight="11055" xr2:uid="{5A634DFE-2E40-48B4-941D-BCCC518AD939}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="31">
   <si>
     <t>Train</t>
   </si>
@@ -75,16 +75,76 @@
   </si>
   <si>
     <t>4th iteration - 60/20/20 split - new background images</t>
+  </si>
+  <si>
+    <t>after robo flow</t>
+  </si>
+  <si>
+    <t>reef</t>
+  </si>
+  <si>
+    <t>bowline</t>
+  </si>
+  <si>
+    <t>bowline_1</t>
+  </si>
+  <si>
+    <t>bowline_2</t>
+  </si>
+  <si>
+    <t>bowline_3</t>
+  </si>
+  <si>
+    <t>bowline_4</t>
+  </si>
+  <si>
+    <t>bowline_5</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Epochs</t>
+  </si>
+  <si>
+    <t>Workers</t>
+  </si>
+  <si>
+    <t>yolov5n</t>
+  </si>
+  <si>
+    <t>yolov5s</t>
+  </si>
+  <si>
+    <t>yolov5m</t>
+  </si>
+  <si>
+    <t>yolov5l</t>
+  </si>
+  <si>
+    <t>yolov5x</t>
+  </si>
+  <si>
+    <t>Time Taken in Seconds</t>
+  </si>
+  <si>
+    <t>out of memory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -426,20 +486,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A70554-815B-442B-91BE-D79E2B4633AC}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -453,7 +516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -468,7 +531,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -483,7 +546,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -498,7 +561,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -513,7 +576,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -528,7 +591,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>SUM(B3:B7)</f>
         <v>318</v>
@@ -546,12 +609,12 @@
         <v>458</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -565,7 +628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -583,7 +646,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -601,7 +664,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -619,7 +682,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -637,7 +700,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -655,7 +718,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>SUM(B12:B16)</f>
         <v>739</v>
@@ -673,12 +736,12 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>0</v>
       </c>
@@ -692,7 +755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -712,7 +775,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -732,7 +795,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -751,7 +814,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -770,7 +833,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -789,7 +852,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <f>SUM(B21:B25)</f>
         <v>681</v>
@@ -807,12 +870,12 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>0</v>
       </c>
@@ -826,7 +889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -846,7 +909,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -866,7 +929,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -886,7 +949,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -906,7 +969,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -925,7 +988,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35">
         <f>SUM(B30:B34)</f>
         <v>967</v>
@@ -943,7 +1006,433 @@
         <v>1615</v>
       </c>
     </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <v>342</v>
+      </c>
+      <c r="C38">
+        <f>228/2</f>
+        <v>114</v>
+      </c>
+      <c r="D38">
+        <f>230/2</f>
+        <v>115</v>
+      </c>
+      <c r="E38">
+        <f>SUM(B38:D38)</f>
+        <v>571</v>
+      </c>
+      <c r="G38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38">
+        <f>776/2</f>
+        <v>388</v>
+      </c>
+      <c r="I38">
+        <f>258/2</f>
+        <v>129</v>
+      </c>
+      <c r="J38">
+        <f>262/2</f>
+        <v>131</v>
+      </c>
+      <c r="K38">
+        <f>SUM(H38:J38)</f>
+        <v>648</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <f>718/2</f>
+        <v>359</v>
+      </c>
+      <c r="C39">
+        <f>238/2</f>
+        <v>119</v>
+      </c>
+      <c r="D39">
+        <f>242/2</f>
+        <v>121</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ref="E39:E43" si="4">SUM(B39:D39)</f>
+        <v>599</v>
+      </c>
+      <c r="G39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39">
+        <f>618/2</f>
+        <v>309</v>
+      </c>
+      <c r="I39">
+        <f>206/2</f>
+        <v>103</v>
+      </c>
+      <c r="J39">
+        <f>206/2</f>
+        <v>103</v>
+      </c>
+      <c r="K39">
+        <f t="shared" ref="K39:K43" si="5">SUM(H39:J39)</f>
+        <v>515</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <f>654/2</f>
+        <v>327</v>
+      </c>
+      <c r="C40">
+        <f>218/2</f>
+        <v>109</v>
+      </c>
+      <c r="D40">
+        <v>110</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="4"/>
+        <v>546</v>
+      </c>
+      <c r="G40" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40">
+        <f>614/2</f>
+        <v>307</v>
+      </c>
+      <c r="I40">
+        <f>204/2</f>
+        <v>102</v>
+      </c>
+      <c r="J40">
+        <v>103</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="5"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <f>590/2</f>
+        <v>295</v>
+      </c>
+      <c r="C41">
+        <f>196/2</f>
+        <v>98</v>
+      </c>
+      <c r="D41">
+        <f>198/2</f>
+        <v>99</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="4"/>
+        <v>492</v>
+      </c>
+      <c r="G41" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41">
+        <f>726/2</f>
+        <v>363</v>
+      </c>
+      <c r="I41">
+        <f>242/2</f>
+        <v>121</v>
+      </c>
+      <c r="J41">
+        <f>242/2</f>
+        <v>121</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="5"/>
+        <v>605</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <f>730/2</f>
+        <v>365</v>
+      </c>
+      <c r="C42">
+        <f>242/2</f>
+        <v>121</v>
+      </c>
+      <c r="D42">
+        <f>246/2</f>
+        <v>123</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="4"/>
+        <v>609</v>
+      </c>
+      <c r="G42" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42">
+        <f>750/2</f>
+        <v>375</v>
+      </c>
+      <c r="I42">
+        <f>250/2</f>
+        <v>125</v>
+      </c>
+      <c r="J42">
+        <f>252/2</f>
+        <v>126</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="5"/>
+        <v>626</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f>SUM(B38:B42)</f>
+        <v>1688</v>
+      </c>
+      <c r="C43">
+        <f>SUM(C38:C42)</f>
+        <v>561</v>
+      </c>
+      <c r="D43">
+        <f>SUM(D38:D42)</f>
+        <v>568</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="4"/>
+        <v>2817</v>
+      </c>
+      <c r="H43">
+        <f>SUM(H38:H42)</f>
+        <v>1742</v>
+      </c>
+      <c r="I43">
+        <f>SUM(I38:I42)</f>
+        <v>580</v>
+      </c>
+      <c r="J43">
+        <f>SUM(J38:J42)</f>
+        <v>584</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="5"/>
+        <v>2906</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>8</v>
+      </c>
+      <c r="D49">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <f>21*60</f>
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+      <c r="C55">
+        <v>8</v>
+      </c>
+      <c r="D55" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <f>44*60</f>
+        <v>2640</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>